<commit_message>
Added 595mm led variant.
</commit_message>
<xml_diff>
--- a/570nm/BOM_JLCPCB_570nm.xlsx
+++ b/570nm/BOM_JLCPCB_570nm.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">C440520</t>
+    <t xml:space="preserve">C188729</t>
   </si>
 </sst>
 </file>
@@ -346,7 +346,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Set resistors in BOM for 570 and 595 led boards.
</commit_message>
<xml_diff>
--- a/570nm/BOM_JLCPCB_570nm.xlsx
+++ b/570nm/BOM_JLCPCB_570nm.xlsx
@@ -92,7 +92,7 @@
     <t xml:space="preserve">C145956</t>
   </si>
   <si>
-    <t xml:space="preserve">resistor, 13 Ohm,  1%  </t>
+    <t xml:space="preserve">resistor, 82 Ohm,  1%  </t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">0603</t>
   </si>
   <si>
-    <t xml:space="preserve">C22798</t>
+    <t xml:space="preserve">C23255 </t>
   </si>
   <si>
     <t xml:space="preserve">LED (570nm)</t>
@@ -346,7 +346,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>